<commit_message>
Bugfix: Changing VehicleTemplate.xlsx row and collumn width
</commit_message>
<xml_diff>
--- a/bin/constants/VehicleTemplate.xlsx
+++ b/bin/constants/VehicleTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VehicleParts\server\bin\constants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF5A09C-93C7-4FCC-913B-62973A5CE053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103D52C0-9514-46EB-8C0D-CA75EC5F4A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
@@ -428,21 +428,25 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" activeCellId="1" sqref="D1:D1048576 E1:E1048576"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="17.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="1" customWidth="1"/>
     <col min="4" max="5" width="8.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="1" customWidth="1"/>
-    <col min="7" max="9" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
     <col min="11" max="11" width="18.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" style="1" customWidth="1"/>
     <col min="13" max="13" width="8.5703125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="20" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="22.140625" style="1" customWidth="1"/>
     <col min="16" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Feat: Added Downloading Result List
</commit_message>
<xml_diff>
--- a/bin/constants/VehicleTemplate.xlsx
+++ b/bin/constants/VehicleTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VehicleParts\server\bin\constants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103D52C0-9514-46EB-8C0D-CA75EC5F4A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67BCD39-562F-42A9-8476-72B7129CE6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,7 +428,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Bugfix: VehicleTemplate doesn't show No collumn number after 3 digits
</commit_message>
<xml_diff>
--- a/bin/constants/VehicleTemplate.xlsx
+++ b/bin/constants/VehicleTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VehicleParts\server\bin\constants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1B6A13-76F2-4976-9375-11E53F49644E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1ACBAE-0883-41B4-BF4D-914332E2217E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
@@ -431,12 +431,12 @@
   <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" style="1" customWidth="1"/>

</xml_diff>

<commit_message>
Bugfix: Download Part List not handling out data, PDF crashes upon logging
</commit_message>
<xml_diff>
--- a/bin/constants/VehicleTemplate.xlsx
+++ b/bin/constants/VehicleTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VehicleParts\server\bin\constants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1ACBAE-0883-41B4-BF4D-914332E2217E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60389B01-0197-40DA-9BEB-DD9579ADCF44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
   <cols>
     <col min="1" max="1" width="7.140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" style="1" customWidth="1"/>
     <col min="5" max="6" width="8.5703125" style="3" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" customWidth="1"/>

</xml_diff>